<commit_message>
Update models performance metrics.xlsx
</commit_message>
<xml_diff>
--- a/models performance metrics.xlsx
+++ b/models performance metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Derrick\Documents\School\Machine Learning\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD313D7E-71AD-47FC-B228-80A7E37BEAA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4122405B-64D2-4D5F-A85D-65C158B2FF5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="765" windowWidth="16575" windowHeight="18480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11460" yWindow="1260" windowWidth="16575" windowHeight="18480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Training Metrics" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="27">
   <si>
     <t>ANN</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>not worth</t>
+  </si>
+  <si>
+    <t>Testing trained models on our dataset</t>
+  </si>
+  <si>
+    <t>Training the models on our dataset</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1398,29 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34:J37">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J34:J38">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1451,8 +1479,313 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34:J37">
-    <cfRule type="colorScale" priority="2">
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AFC82E-723D-4D59-9572-2BCAF5C341F6}">
+  <dimension ref="B5:I39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="H8">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.96879999999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.27560000000000001</v>
+      </c>
+      <c r="H9">
+        <v>287896</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.19059999999999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>2.1709999999999998</v>
+      </c>
+      <c r="H10">
+        <v>76840</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.90939999999999999</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.46789999999999998</v>
+      </c>
+      <c r="H11">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.98750000000000004</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.18129999999999999</v>
+      </c>
+      <c r="H18">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.60000002384185702</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1.788</v>
+      </c>
+      <c r="H19">
+        <v>144011</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.89690000000000003</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.42720000000000002</v>
+      </c>
+      <c r="H21">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="F26" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.66279071569442705</v>
+      </c>
+      <c r="G27" s="1">
+        <v>9.7774999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.41860464215278598</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4.9439000000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0.11627907305955799</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2.0794999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.62790697813034002</v>
+      </c>
+      <c r="G30" s="1">
+        <v>5.1040999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8">
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0.1201</v>
+      </c>
+      <c r="G36" s="1">
+        <v>2.0933000000000002</v>
+      </c>
+      <c r="H36">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.98970000000000002</v>
+      </c>
+      <c r="G37" s="1">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="H37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.1298</v>
+      </c>
+      <c r="G38" s="1">
+        <v>2.0783</v>
+      </c>
+      <c r="H38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.89534884691238403</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="H39">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F8:F11">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1463,8 +1796,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J34:J38">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="F18:F21">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1475,184 +1808,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6AFC82E-723D-4D59-9572-2BCAF5C341F6}">
-  <dimension ref="B5:I21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="5" spans="2:8">
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.97499999999999998</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="H8">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.96879999999999999</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0.27560000000000001</v>
-      </c>
-      <c r="H9">
-        <v>287896</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.19059999999999999</v>
-      </c>
-      <c r="G10" s="1">
-        <v>2.1709999999999998</v>
-      </c>
-      <c r="H10">
-        <v>76840</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.90939999999999999</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.46789999999999998</v>
-      </c>
-      <c r="H11">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="D16" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9">
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9">
-      <c r="B18" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0.98750000000000004</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0.18129999999999999</v>
-      </c>
-      <c r="H18">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9">
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0.60000002384185702</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1.788</v>
-      </c>
-      <c r="H19">
-        <v>144011</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9">
-      <c r="B20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" t="s">
-        <v>23</v>
-      </c>
-      <c r="I20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9">
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0.89690000000000003</v>
-      </c>
-      <c r="G21" s="1">
-        <v>0.42720000000000002</v>
-      </c>
-      <c r="H21">
-        <v>280</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="F8:F11">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="F20">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1664,7 +1821,31 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8:G11">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:G21">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G20">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1676,31 +1857,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H8:H11">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F20">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G20">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1712,31 +1869,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H18:H21 I20">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F21">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18:G21">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>